<commit_message>
QA-7808 fixes for import cases and case search
</commit_message>
<xml_diff>
--- a/HQSmokeTests/userInputs/test_data/reassign_cases.xlsx
+++ b/HQSmokeTests/userInputs/test_data/reassign_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsi-user\Documents\Master Scripts\HQSmokeTests\userInputs\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsi-user\PycharmProjects\New Structure\dimagi-qa\HQSmokeTests\userInputs\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5467696-F558-4F46-8218-2C175CF832DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FBE746-5F3A-4FD5-95BA-525A8EFFA938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>caseid</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>owner_name</t>
-  </si>
-  <si>
-    <t>2cb336a7-b959-45a4-8619-0b1dbad28321</t>
   </si>
   <si>
     <t>aashiyan</t>
@@ -389,17 +386,17 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,21 +416,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>